<commit_message>
Add daily scrum log and updated burndown
</commit_message>
<xml_diff>
--- a/admin/9-JulSprintBurndown.xlsx
+++ b/admin/9-JulSprintBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBADC4FD-9777-4C86-80A9-9F249811DB88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA1973-AAF2-427C-B00C-C1272F6C0B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16275" yWindow="-15525" windowWidth="24075" windowHeight="15165" xr2:uid="{E7DD3797-FEF2-40B3-90F6-28EA74433530}"/>
   </bookViews>
@@ -488,13 +488,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,7 +1604,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1698,11 +1698,11 @@
         <v>5</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="7">
         <f>$B$4-SUM($D$7:D8)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="E9" s="7">
         <f>$B$4-SUM($D$7:D9)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="E10" s="7">
         <f>$B$4-SUM($D$7:D10)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="E12" s="2">
         <f>E7-E10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>